<commit_message>
Update: Subir cuadernillo estadísticas descriptivas final y corregir nombres de variables de variables municipales adicionales
</commit_message>
<xml_diff>
--- a/datos_adicionales/poblacion2020.xlsx
+++ b/datos_adicionales/poblacion2020.xlsx
@@ -5,10 +5,10 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jose.nino\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jose.nino\Documents\Git taller datos abiertos\taller_datos_abiertos_ICBF\datos_adicionales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC8BBB52-B658-49B6-B02A-B67BD07673CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CFDEC2B-392F-4EEC-8EDF-09FA7A5EBD03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3405,16 +3405,16 @@
     <t>99773</t>
   </si>
   <si>
-    <t>CabeceraMunicipal_2021</t>
-  </si>
-  <si>
-    <t>CentrosPoblados _RuralDisperso_2021</t>
-  </si>
-  <si>
-    <t>PobTotal_2021</t>
-  </si>
-  <si>
-    <t>PorcentajeRural_2021</t>
+    <t>CabeceraMunicipal_2020</t>
+  </si>
+  <si>
+    <t>CentrosPoblados _RuralDisperso_2020</t>
+  </si>
+  <si>
+    <t>PobTotal_2020</t>
+  </si>
+  <si>
+    <t>PorcentajeRural_2020</t>
   </si>
 </sst>
 </file>
@@ -3787,7 +3787,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BEA2BD9-F605-4707-942E-A22640AAFE1B}">
   <dimension ref="A1:E1123"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>